<commit_message>
+ Fixed some dead copper.
</commit_message>
<xml_diff>
--- a/Altium_prj/Project Outputs for CAN_CurrentLoopModule/BOM/Bill of Materials-CAN_CurrentLoopModule.xlsx
+++ b/Altium_prj/Project Outputs for CAN_CurrentLoopModule/BOM/Bill of Materials-CAN_CurrentLoopModule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\CANOPEN_CURRENT_MODULE\trunk\HW\Altium_prj\Project Outputs for CAN_CurrentLoopModule\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCD63571-5C9E-4C29-BDE8-59006C888807}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFEA066D-4D4E-4155-AAFA-9F1590132428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="1755" windowWidth="21600" windowHeight="11385" xr2:uid="{3817749E-1974-4866-ABDD-AF92F81FBCDB}"/>
+    <workbookView xWindow="2115" yWindow="1755" windowWidth="21600" windowHeight="11385" xr2:uid="{1E4091FD-ADB6-46BE-8EE9-06A5C4A45B7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-CAN_CurrentLo" sheetId="1" r:id="rId1"/>
@@ -780,7 +780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0334DD27-0D84-46D9-9CA6-17D417E980E1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E70E22-3D78-4D84-B926-6543A22801AC}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>

<commit_message>
+ Fixed distances between pad/via/trace and GND pours.
</commit_message>
<xml_diff>
--- a/Altium_prj/Project Outputs for CAN_CurrentLoopModule/BOM/Bill of Materials-CAN_CurrentLoopModule.xlsx
+++ b/Altium_prj/Project Outputs for CAN_CurrentLoopModule/BOM/Bill of Materials-CAN_CurrentLoopModule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\CANOPEN_CURRENT_MODULE\trunk\HW\Altium_prj\Project Outputs for CAN_CurrentLoopModule\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFEA066D-4D4E-4155-AAFA-9F1590132428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{37AAA0A8-F4E6-4D84-912A-E9A772CA76F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="1755" windowWidth="21600" windowHeight="11385" xr2:uid="{1E4091FD-ADB6-46BE-8EE9-06A5C4A45B7E}"/>
+    <workbookView xWindow="2115" yWindow="1755" windowWidth="21600" windowHeight="11385" xr2:uid="{B1DBC44C-A342-4F40-BC0E-B09EFAD3505C}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-CAN_CurrentLo" sheetId="1" r:id="rId1"/>
@@ -780,7 +780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E70E22-3D78-4D84-B926-6543A22801AC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A03C37A-A9F5-4996-AE0D-D3067DFAAC2F}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>